<commit_message>
Oragene saliva father app added
</commit_message>
<xml_diff>
--- a/HairSampleMother/DB and Documents/HairSample.xlsx
+++ b/HairSampleMother/DB and Documents/HairSample.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Questions" sheetId="2" r:id="rId1"/>
@@ -1817,7 +1817,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:V78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="V2" sqref="V2:V18"/>
     </sheetView>
   </sheetViews>
@@ -3018,7 +3018,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G1291"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="G2" sqref="G2:G24"/>
     </sheetView>
   </sheetViews>
@@ -3305,11 +3305,11 @@
         <v>1</v>
       </c>
       <c r="F14" s="37" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="G14" s="35" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('13','q11', '1. All','','1','q13');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('13','q11', '1. All','','1','END');</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="15" customFormat="1" ht="15">

</xml_diff>